<commit_message>
Stand am 04.04.2022 - Mails gefixt
</commit_message>
<xml_diff>
--- a/DemoNovaland/Programme/TabellenWerte Novaland Excel Tabelle.xlsx
+++ b/DemoNovaland/Programme/TabellenWerte Novaland Excel Tabelle.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Novaland Stuff\TabellenWerte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DemoNovaland\DemoNovaland\Programme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC17695-139D-4E13-9C71-BB7790FBF0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC04C1BD-429A-425A-A602-5275759E19C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6FFC6BF0-694B-4E8C-B697-64E5C16476E9}"/>
   </bookViews>
@@ -1546,8 +1546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE96E53-20C1-4A82-BCCB-6DAAE384CEF1}">
   <dimension ref="A1:F179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="B160" sqref="B160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>